<commit_message>
fixed unicode /u0001 escaping issue with php < v5.4
</commit_message>
<xml_diff>
--- a/BacklogTasks.xlsx
+++ b/BacklogTasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Display message to registered users who have not yet paid</t>
   </si>
@@ -76,13 +76,31 @@
   </si>
   <si>
     <t>Refactor DAL - include disconnects, monitor performance</t>
+  </si>
+  <si>
+    <t>Fix footer - change to navbar</t>
+  </si>
+  <si>
+    <t>Fix header navbar (white highlight on middle 2 buttons)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Fix "History for... " injection of username</t>
+  </si>
+  <si>
+    <t>Add "Full name" field to registration a</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +108,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,13 +138,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,7 +450,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +460,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
@@ -438,7 +474,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2">
@@ -447,120 +483,123 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -568,24 +607,24 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
@@ -593,16 +632,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -610,22 +646,84 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>SUM(C2:C22)</f>
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D21">
+    <sortCondition ref="A2:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>